<commit_message>
fix du bug dans l'affichage ensemble
</commit_message>
<xml_diff>
--- a/Notes & Documentations/Dernier_Mandat.xlsx
+++ b/Notes & Documentations/Dernier_Mandat.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>alll activities pour ecran styliste</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>David</t>
+  </si>
+  <si>
+    <t>godard</t>
+  </si>
+  <si>
+    <t>gab</t>
+  </si>
+  <si>
+    <t>fini</t>
   </si>
 </sst>
 </file>
@@ -88,7 +97,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -103,7 +111,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -122,8 +130,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,92 +412,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H14"/>
+  <dimension ref="A2:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="H4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="H6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
       <c r="H10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="H14" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
im fucking tired of this shit
</commit_message>
<xml_diff>
--- a/Notes & Documentations/Dernier_Mandat.xlsx
+++ b/Notes & Documentations/Dernier_Mandat.xlsx
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ok .. max is weird
</commit_message>
<xml_diff>
--- a/Notes & Documentations/Dernier_Mandat.xlsx
+++ b/Notes & Documentations/Dernier_Mandat.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>alll activities pour ecran styliste</t>
   </si>
@@ -414,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,6 +532,9 @@
       <c r="A11" t="s">
         <v>7</v>
       </c>
+      <c r="H11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -552,11 +555,19 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
       <c r="H13" t="s">
         <v>13</v>
+      </c>
+      <c r="I13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -571,6 +582,9 @@
       <c r="H14" t="s">
         <v>16</v>
       </c>
+      <c r="I14" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>